<commit_message>
modify statistic info about datasets
</commit_message>
<xml_diff>
--- a/statistic/final.xlsx
+++ b/statistic/final.xlsx
@@ -558,10 +558,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">   84.95+1.15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>74.26+2.51</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -675,6 +671,10 @@
   </si>
   <si>
     <t>81.77+3.45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>85.49+1.09</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1056,7 +1056,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>35</v>
@@ -1167,7 +1167,7 @@
         <v>24</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>132</v>
@@ -1202,7 +1202,7 @@
         <v>31</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>104</v>
@@ -1245,16 +1245,16 @@
         <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>41</v>
@@ -1309,19 +1309,19 @@
         <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>125</v>
@@ -1338,10 +1338,10 @@
         <v>53</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>114</v>
@@ -1362,7 +1362,7 @@
         <v>57</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1373,7 +1373,7 @@
         <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>115</v>
@@ -1382,10 +1382,10 @@
         <v>59</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>127</v>
@@ -1402,7 +1402,7 @@
         <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>133</v>
@@ -1411,13 +1411,13 @@
         <v>116</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>128</v>
@@ -1440,7 +1440,7 @@
         <v>107</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>67</v>
@@ -1466,22 +1466,22 @@
         <v>72</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>122</v>
@@ -1504,7 +1504,7 @@
         <v>79</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>76</v>
@@ -1516,7 +1516,7 @@
         <v>77</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
Paper is modified by YongLiu and JianLi has tried a lot on the experiment part
</commit_message>
<xml_diff>
--- a/statistic/final.xlsx
+++ b/statistic/final.xlsx
@@ -22,22 +22,330 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="164">
   <si>
+    <t>1vRest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C&amp;S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>76.77+2.42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>77.14+2.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>psortPos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>73.33+4.21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>71.70+4.89</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>73.55+4.22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74.41+3.55</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74.07+2.16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74.66+1.90</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>77.78+1.52</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>77.49+1.53</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>78.35+1.46</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>segment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>96.87+0.80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vehicle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>81.57+2.24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>77.28+2.78</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>97.24+3.05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>98.52+1.89</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>95.89+0.56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>96.3+0.79</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>glass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>72.46+6.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iris</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>96.76+2.63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>96.11+4.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>83.84+4.21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>satimage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70.70+4.89</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dna</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>feature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>glass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>satimage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>segment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>svmguide2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>svmguide4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vehicle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vowel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>psortPos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>psortNeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nonpl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>92.15+2.57</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>98.00+2.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>79.35+2.27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75.16+1.48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75.61+3.56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>92.02+1.50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>82.72+1.92</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>93.16+0.66</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>83.16+3.63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>77.60+2.63</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>71.87+4.87</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>98.61+1.75</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74.96+2.93</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>72.83+2.20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   84.95+1.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>85.17+3.83</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>97.04+1.85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>62.32+4.97</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>98.55+1.13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>99.44+1.13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>95.61+0.73</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>99.63+0.96</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>96.08+0.83</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>71.98+5.75</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>71.24+8.14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>84.27+3.03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SG-MKL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1v1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1vRest</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C&amp;S</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GMNP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>MC-MKL p=1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MC-MKL p=2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>UFO-MKL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -46,6 +354,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>78.01+2.17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70.12+2.96</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>75.83+2.69</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -54,10 +370,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>70.12+2.96</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>75.42+3.64</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -66,27 +378,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>76.77+2.42</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>77.14+2.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>psortPos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>73.33+4.21</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>71.70+4.89</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>73.55+4.22</t>
+    <t>76.23+3.39</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>63.85+3.94</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -94,75 +390,67 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>74.41+3.55</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>76.23+3.39</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>psortNeg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>57.85+2.49</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>73.74+2.87</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>71.94+2.50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74.27+2.51</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>72.42+2.65</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>73.80+2.26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>nonpl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>78.69+1.58</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>79.15+1.51</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>77.89+1.79</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>77.95+1.64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>78.07+1.56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>sector</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>73.74+2.87</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>71.94+2.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>72.42+2.65</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>73.80+2.26</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74.07+2.16</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74.66+1.90</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>77.78+1.52</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>77.49+1.53</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>78.35+1.46</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>78.07+1.56</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>79.15+1.51</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>78.01+2.17</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CONV</t>
+    <t>93.39+0.70</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>92.83+2.62</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -170,15 +458,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>93.34+0.61</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>92.60+0.47</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>93.39+0.70</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>segment</t>
+    <t>97.62+0.83</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>96.79+0.91</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>95.07+1.11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -186,7 +482,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>96.87+0.80</t>
+    <t>97.02+0.65</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>96.98+0.64</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -194,15 +494,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>97.2+0.82</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>97.62+0.83</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vehicle</t>
+    <t>97.20+0.82</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>85.11+1.94</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>76.27+3.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>76.92+2.83</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -210,15 +514,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>81.57+2.24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>76.92+2.83</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>77.28+2.78</t>
+    <t>98.83+5.57</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>98.12+1.76</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>98.22+1.83</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>98.27+1.22</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -230,15 +538,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>98.83+5.57</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wine</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>97.24+3.05</t>
+    <t>99.63+0.96</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>97.87+2.80</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -250,15 +554,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>98.52+1.89</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dna</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>95.89+0.56</t>
+    <t>94.6+0.94</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>96.27+0.68</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -270,11 +570,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>96.3+0.79</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>glass</t>
+    <t>73.72+5.80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75.19+5.05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>63.95+6.04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70.00+5.75</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>69.07+8.08</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -282,15 +594,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>72.46+6.12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>iris</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>96.76+2.63</t>
+    <t>97.33+2.53</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>89.67+8.71</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>96.11+3.04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>96.00+3.65</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>95.44+3.66</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -298,23 +622,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>96.11+4.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>95.44+3.66</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>97.33+2.53</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>svmguide2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>83.84+4.21</t>
+    <t>82.69+5.65</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>81.10+4.15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>84.79+3.45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>81.77+3.45</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -322,7 +646,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>satimage</t>
+    <t>91.78+0.82</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>90.86+1.07</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -330,351 +658,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>89.29+0.96</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>89.97+0.81</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>92.27+0.98</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>90.43+1.27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>91.92+0.83</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>90.86+1.07</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>91.78+0.82</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>81.24+2.21</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>96.11+3.04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>89.29+0.96</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>78.69+1.58</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>70.70+4.89</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>90.43+1.27</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dna</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>class</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>feature</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>glass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>satimage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sector</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>segment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>svmguide2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>svmguide4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vehicle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vowel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wine</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>plant</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>psortPos</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>psortNeg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nonpl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>77.95+1.64</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>92.83+2.62</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>92.15+2.57</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>98.00+2.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>79.35+2.27</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>93.34+0.61</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>63.85+3.94</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>57.85+2.49</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>75.16+1.48</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>75.61+3.56</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>97.87+2.80</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>92.02+1.50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>63.95+6.04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>82.72+1.92</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>76.27+3.15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>93.16+0.66</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MC-MKL p=2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MC-MKL p=1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>83.16+3.63</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>77.60+2.63</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>71.87+4.87</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>98.27+1.22</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>98.61+1.75</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>96.27+0.68</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>69.07+8.08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>96.00+3.65</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74.96+2.93</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>96.98+0.64</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>72.83+2.20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>75.19+5.05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   84.95+1.15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74.26+2.51</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>85.17+3.83</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>77.89+1.79</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>97.04+1.85</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>92.27+0.98</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>62.32+4.97</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>98.12+1.76</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>98.22+1.83</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>96.78+0.91</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>95.07+1.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>97.02+0.65</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SG-MKL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>98.55+1.13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>99.44+1.13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>95.61+0.73</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>99.63+0.96</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>99.63+0.96</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>94.6+0.94</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>96.08+0.83</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>73.72+5.80</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>71.98+5.75</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>71.24+8.14</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>70.00+5.75</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>89.67+8.71</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>80.25+4.04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>84.79+3.45</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>84.27+3.03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>81.10+4.15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>81.77+3.45</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -682,7 +682,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -722,6 +722,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -743,7 +752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -761,6 +770,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1046,7 +1067,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1056,473 +1077,473 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>146</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>121</v>
+        <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>123</v>
+        <v>58</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>124</v>
+        <v>59</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>93</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>135</v>
+        <v>95</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>132</v>
+        <v>62</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>25</v>
+        <v>97</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>109</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>81</v>
+        <v>55</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>130</v>
+        <v>61</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>122</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>123</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>147</v>
+        <v>67</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>140</v>
+        <v>66</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>138</v>
+        <v>65</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>50</v>
+        <v>127</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>55</v>
+        <v>131</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>56</v>
+        <v>132</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>126</v>
+        <v>60</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>148</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>153</v>
+        <v>71</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>115</v>
+        <v>54</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>149</v>
+        <v>69</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>60</v>
+        <v>135</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>155</v>
+        <v>72</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>156</v>
+        <v>73</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>64</v>
+        <v>142</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>71</v>
+        <v>143</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>144</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>70</v>
+        <v>148</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>161</v>
+        <v>74</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>122</v>
+        <v>57</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>74</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>80</v>
+        <v>30</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>76</v>
+        <v>158</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>83</v>
+        <v>159</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>139</v>
+        <v>160</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>78</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1570,18 +1591,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -1592,7 +1613,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -1603,7 +1624,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -1614,7 +1635,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -1625,7 +1646,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1639,7 +1660,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1653,7 +1674,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1667,7 +1688,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -1681,7 +1702,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="B10">
         <v>105</v>
@@ -1695,7 +1716,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -1709,7 +1730,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -1723,7 +1744,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1737,7 +1758,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -1751,7 +1772,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>11</v>
@@ -1765,7 +1786,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>3</v>

</xml_diff>

<commit_message>
some changes on supplementary
</commit_message>
<xml_diff>
--- a/statistic/final.xlsx
+++ b/statistic/final.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9570" windowHeight="7140"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="1" r:id="rId1"/>
@@ -650,10 +650,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>90.86+1.07</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>90.67+0.91</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -666,15 +662,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>92.27+0.98</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>90.43+1.27</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>91.92+0.83</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>91.86+0.62</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>91.64+0.88</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1067,7 +1067,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1518,32 +1518,32 @@
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="10" t="s">
         <v>156</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1580,7 +1580,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D10"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>